<commit_message>
update tag add interface
</commit_message>
<xml_diff>
--- a/Interface Data Structure.xlsx
+++ b/Interface Data Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\Course\Mobile Computing\Assignment\COMP90018-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0082381B-99F0-4979-827E-398AABE7CFD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A93FFA-39DC-4F97-9EEB-DC89C6F4BB56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="0" windowWidth="17085" windowHeight="15600" tabRatio="947" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="947" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="17" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="168">
   <si>
     <t>RegisterRequest</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -680,6 +680,34 @@
   </si>
   <si>
     <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createUser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1011,7 +1039,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1060,6 +1088,9 @@
       <c r="A6" t="s">
         <v>120</v>
       </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1073,10 +1104,16 @@
       <c r="A8" t="s">
         <v>122</v>
       </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,7 +1167,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1380,9 +1417,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28829E08-9E60-4718-AFBE-5C652A342AD9}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1529,39 +1568,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>87</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -1569,34 +1608,23 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2839,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C521DD-7841-4D1A-80FC-84BB75D93D93}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3139,10 +3167,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB5CDCC-35D6-481E-8D3F-990341E52EB1}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3315,46 +3343,69 @@
         <v>153</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>